<commit_message>
update for the file list control
</commit_message>
<xml_diff>
--- a/pico_pack/file_list_free.xlsx
+++ b/pico_pack/file_list_free.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20407"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\py_gary\py_pico\pico_pack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6ED349F-3EBC-4F5F-B0B9-3EA4D9BC564F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F007A546-8604-4495-9AB2-66C9A66449BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -419,21 +419,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.0703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="84.92578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="85.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.640625" customWidth="1"/>
+    <col min="1" max="1" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.25" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -447,60 +447,60 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>